<commit_message>
added extensive tests to experimental parser
</commit_message>
<xml_diff>
--- a/tests/data/20250114_experiment_file.xlsx
+++ b/tests/data/20250114_experiment_file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="148">
   <si>
     <t xml:space="preserve">Experiment Info</t>
   </si>
@@ -127,63 +127,66 @@
     <t xml:space="preserve">Solvent 1 volume [uL]</t>
   </si>
   <si>
+    <t xml:space="preserve">Solute 1 name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solute 1 Concentration [mM]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solution volume [um]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spin Delay [s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotation speed 1 [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotation time 1 [s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acceleration 1 [rpm/s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotation speed 2 [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotation time 2 [s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acceleration 2 [rpm/s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anti solvent name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anti solvent volume [ml]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anti solvent dropping time [s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anti solvent dropping speed [ul/s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anti solvent dropping heigt [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annealing time [min]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annealing temperature [°C]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annealing athmosphere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Solute 1 type</t>
   </si>
   <si>
-    <t xml:space="preserve">Solute 1 Concentration [mM]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solution volume [um]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spin Delay [s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rotation speed 1 [rpm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rotation time 1 [s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acceleration 1 [rpm/s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rotation speed 2 [rpm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rotation time 2 [s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acceleration 2 [rpm/s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anti solvent name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anti solvent volume [ml]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anti solvent dropping time [s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anti solvent dropping speed [ul/s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anti solvent dropping heigt [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annealing time [min]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annealing temperature [°C]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annealing athmosphere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Solute 2 type</t>
   </si>
   <si>
@@ -310,10 +313,10 @@
     <t xml:space="preserve">Base pressure [bar]</t>
   </si>
   <si>
-    <t xml:space="preserve">Pressure start [bar]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pressure end [bar]</t>
+    <t xml:space="preserve">Pressure start [mbar]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressure end [mbar]</t>
   </si>
   <si>
     <t xml:space="preserve">Source temperature start[°C]</t>
@@ -640,11 +643,11 @@
   </sheetPr>
   <dimension ref="A1:EJ31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BW1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CG2" activeCellId="0" sqref="CG2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="DC1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="DN2" activeCellId="0" sqref="DN2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14"/>
@@ -1094,52 +1097,52 @@
         <v>34</v>
       </c>
       <c r="AX2" s="2" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="AY2" s="2" t="s">
         <v>36</v>
       </c>
       <c r="AZ2" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="BA2" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="BB2" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="BC2" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="BD2" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="BE2" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BF2" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="BG2" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="BH2" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="BI2" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="BJ2" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="BK2" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="BL2" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="BM2" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="BN2" s="2" t="s">
         <v>50</v>
@@ -1163,64 +1166,64 @@
         <v>32</v>
       </c>
       <c r="BU2" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BV2" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="BW2" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="BX2" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="BY2" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="BZ2" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="CA2" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="CB2" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="CC2" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="CD2" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="CE2" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="CF2" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="CG2" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="CH2" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="CI2" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="CJ2" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="CK2" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="CL2" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="CM2" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="CN2" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="CO2" s="2" t="s">
         <v>30</v>
@@ -1238,7 +1241,7 @@
         <v>34</v>
       </c>
       <c r="CT2" s="2" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="CU2" s="2" t="s">
         <v>36</v>
@@ -1247,25 +1250,25 @@
         <v>37</v>
       </c>
       <c r="CW2" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="CX2" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="CY2" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="CZ2" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="DA2" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="DB2" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="DC2" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="DD2" s="2" t="s">
         <v>50</v>
@@ -1289,34 +1292,34 @@
         <v>32</v>
       </c>
       <c r="DK2" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="DL2" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="DM2" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="DN2" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="DO2" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="DP2" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="DQ2" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="DR2" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="DS2" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="DT2" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="DU2" s="2" t="s">
         <v>53</v>
@@ -1331,37 +1334,37 @@
         <v>32</v>
       </c>
       <c r="DY2" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="DZ2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="EA2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="EB2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="EC2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="ED2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="EE2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="EF2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="EA2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="EB2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="EC2" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="ED2" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="EE2" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="EF2" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="EG2" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="EH2" s="2" t="s">
         <v>53</v>
       </c>
       <c r="EI2" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="EJ2" s="2" t="s">
         <v>53</v>
@@ -1369,10 +1372,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
@@ -1385,22 +1388,22 @@
         <v>hzb_TestP_AA_1_c-1</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>10</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M3" s="0" t="n">
         <v>100</v>
@@ -1409,7 +1412,7 @@
         <v>10</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P3" s="0" t="n">
         <v>10</v>
@@ -1418,7 +1421,7 @@
         <v>100</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S3" s="0" t="n">
         <v>20</v>
@@ -1427,22 +1430,22 @@
         <v>50</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Y3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AA3" s="0" t="n">
         <v>2</v>
@@ -1472,7 +1475,7 @@
         <v>10</v>
       </c>
       <c r="AJ3" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AK3" s="0" t="n">
         <v>10</v>
@@ -1493,40 +1496,40 @@
         <v>100</v>
       </c>
       <c r="AQ3" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AR3" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AS3" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AT3" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AU3" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AV3" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AW3" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AX3" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AY3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AZ3" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BA3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BB3" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BC3" s="0" t="n">
         <v>10</v>
@@ -1535,10 +1538,10 @@
         <v>1</v>
       </c>
       <c r="BE3" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="BF3" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="BG3" s="0" t="n">
         <v>5</v>
@@ -1568,19 +1571,19 @@
         <v>14</v>
       </c>
       <c r="BP3" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BR3" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BS3" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BT3" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BU3" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BV3" s="0" t="n">
         <v>10</v>
@@ -1637,25 +1640,25 @@
         <v>3</v>
       </c>
       <c r="CN3" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="CO3" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="CP3" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="CQ3" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="CR3" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="CS3" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CT3" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="CU3" s="0" t="n">
         <v>10</v>
@@ -1691,19 +1694,19 @@
         <v>5</v>
       </c>
       <c r="DF3" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DH3" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="DI3" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="DJ3" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DK3" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="DL3" s="0" t="n">
         <v>10</v>
@@ -1730,16 +1733,16 @@
         <v>1</v>
       </c>
       <c r="DV3" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="DW3" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="DX3" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DY3" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DZ3" s="0" t="n">
         <v>100</v>
@@ -1766,15 +1769,15 @@
         <v>1</v>
       </c>
       <c r="EI3" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -1787,22 +1790,22 @@
         <v>hzb_TestP_AA_1_c-2</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>10</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M4" s="0" t="n">
         <v>100</v>
@@ -1811,7 +1814,7 @@
         <v>10</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P4" s="0" t="n">
         <v>10</v>
@@ -1820,7 +1823,7 @@
         <v>100</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S4" s="0" t="n">
         <v>20</v>
@@ -1829,22 +1832,22 @@
         <v>50</v>
       </c>
       <c r="U4" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="V4" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="W4" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Y4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="Z4" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AA4" s="0" t="n">
         <v>2</v>
@@ -1874,7 +1877,7 @@
         <v>10</v>
       </c>
       <c r="AJ4" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AK4" s="0" t="n">
         <v>10</v>
@@ -1895,40 +1898,40 @@
         <v>100</v>
       </c>
       <c r="AQ4" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AR4" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AS4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AT4" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AU4" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AV4" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AW4" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AX4" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AY4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AZ4" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BA4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BB4" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BC4" s="0" t="n">
         <v>10</v>
@@ -1937,10 +1940,10 @@
         <v>1</v>
       </c>
       <c r="BE4" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="BF4" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="BG4" s="0" t="n">
         <v>5</v>
@@ -1970,19 +1973,19 @@
         <v>14</v>
       </c>
       <c r="BP4" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BR4" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BS4" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BT4" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BU4" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BV4" s="0" t="n">
         <v>10</v>
@@ -2039,25 +2042,25 @@
         <v>3</v>
       </c>
       <c r="CN4" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="CO4" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="CP4" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="CQ4" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="CR4" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="CS4" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CT4" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="CU4" s="0" t="n">
         <v>10</v>
@@ -2093,19 +2096,19 @@
         <v>5</v>
       </c>
       <c r="DF4" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DH4" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="DI4" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="DJ4" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DK4" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="DL4" s="0" t="n">
         <v>10</v>
@@ -2132,16 +2135,16 @@
         <v>1</v>
       </c>
       <c r="DV4" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="DW4" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="DX4" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DY4" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DZ4" s="0" t="n">
         <v>100</v>
@@ -2168,15 +2171,15 @@
         <v>1</v>
       </c>
       <c r="EI4" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
@@ -2189,22 +2192,22 @@
         <v>hzb_TestP_AA_1_c-3</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>10</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M5" s="0" t="n">
         <v>100</v>
@@ -2213,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P5" s="0" t="n">
         <v>10</v>
@@ -2222,7 +2225,7 @@
         <v>100</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S5" s="0" t="n">
         <v>20</v>
@@ -2231,22 +2234,22 @@
         <v>50</v>
       </c>
       <c r="U5" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="V5" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="W5" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="X5" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Y5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="Z5" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AA5" s="0" t="n">
         <v>2</v>
@@ -2276,7 +2279,7 @@
         <v>10</v>
       </c>
       <c r="AJ5" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AK5" s="0" t="n">
         <v>10</v>
@@ -2297,40 +2300,40 @@
         <v>100</v>
       </c>
       <c r="AQ5" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AR5" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AS5" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AT5" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AU5" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AV5" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AW5" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AX5" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AY5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AZ5" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BA5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BB5" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BC5" s="0" t="n">
         <v>10</v>
@@ -2339,10 +2342,10 @@
         <v>1</v>
       </c>
       <c r="BE5" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="BF5" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="BG5" s="0" t="n">
         <v>5</v>
@@ -2372,19 +2375,19 @@
         <v>14</v>
       </c>
       <c r="BP5" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BR5" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BS5" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BT5" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BU5" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BV5" s="0" t="n">
         <v>10</v>
@@ -2441,25 +2444,25 @@
         <v>3</v>
       </c>
       <c r="CN5" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="CO5" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="CP5" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="CQ5" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="CR5" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="CS5" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CT5" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="CU5" s="0" t="n">
         <v>10</v>
@@ -2495,19 +2498,19 @@
         <v>5</v>
       </c>
       <c r="DF5" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DH5" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="DI5" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="DJ5" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DK5" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="DL5" s="0" t="n">
         <v>10</v>
@@ -2534,16 +2537,16 @@
         <v>1</v>
       </c>
       <c r="DV5" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="DW5" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="DX5" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DY5" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DZ5" s="0" t="n">
         <v>100</v>
@@ -2570,15 +2573,15 @@
         <v>1</v>
       </c>
       <c r="EI5" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
@@ -2591,22 +2594,22 @@
         <v>hzb_TestP_AA_1_c-4</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>10</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M6" s="0" t="n">
         <v>100</v>
@@ -2615,7 +2618,7 @@
         <v>10</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P6" s="0" t="n">
         <v>10</v>
@@ -2624,7 +2627,7 @@
         <v>100</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S6" s="0" t="n">
         <v>20</v>
@@ -2633,22 +2636,22 @@
         <v>50</v>
       </c>
       <c r="U6" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="V6" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="W6" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Y6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="Z6" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AA6" s="0" t="n">
         <v>2</v>
@@ -2678,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="AJ6" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AK6" s="0" t="n">
         <v>10</v>
@@ -2699,40 +2702,40 @@
         <v>100</v>
       </c>
       <c r="AQ6" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AR6" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AS6" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AT6" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AU6" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AV6" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AW6" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AX6" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AY6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AZ6" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BA6" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BB6" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BC6" s="0" t="n">
         <v>10</v>
@@ -2741,10 +2744,10 @@
         <v>1</v>
       </c>
       <c r="BE6" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="BF6" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="BG6" s="0" t="n">
         <v>5</v>
@@ -2774,19 +2777,19 @@
         <v>14</v>
       </c>
       <c r="BP6" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BR6" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BS6" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BT6" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BU6" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BV6" s="0" t="n">
         <v>10</v>
@@ -2843,25 +2846,25 @@
         <v>3</v>
       </c>
       <c r="CN6" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="CO6" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="CP6" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="CQ6" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="CR6" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="CS6" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CT6" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="CU6" s="0" t="n">
         <v>10</v>
@@ -2897,19 +2900,19 @@
         <v>5</v>
       </c>
       <c r="DF6" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DH6" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="DI6" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="DJ6" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DK6" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="DL6" s="0" t="n">
         <v>10</v>
@@ -2936,16 +2939,16 @@
         <v>1</v>
       </c>
       <c r="DV6" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="DW6" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="DX6" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DY6" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DZ6" s="0" t="n">
         <v>100</v>
@@ -2972,15 +2975,15 @@
         <v>1</v>
       </c>
       <c r="EI6" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>1</v>
@@ -2993,22 +2996,22 @@
         <v>hzb_TestP_AA_1_c-5</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>10</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M7" s="0" t="n">
         <v>100</v>
@@ -3017,7 +3020,7 @@
         <v>10</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P7" s="0" t="n">
         <v>10</v>
@@ -3026,7 +3029,7 @@
         <v>100</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S7" s="0" t="n">
         <v>20</v>
@@ -3035,22 +3038,22 @@
         <v>50</v>
       </c>
       <c r="U7" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="V7" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="W7" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="X7" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Y7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="Z7" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AA7" s="0" t="n">
         <v>2</v>
@@ -3080,7 +3083,7 @@
         <v>10</v>
       </c>
       <c r="AJ7" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AK7" s="0" t="n">
         <v>10</v>
@@ -3101,40 +3104,40 @@
         <v>100</v>
       </c>
       <c r="AQ7" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AR7" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AS7" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AT7" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AU7" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AV7" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AW7" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AX7" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AY7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AZ7" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BA7" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BB7" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BC7" s="0" t="n">
         <v>10</v>
@@ -3143,10 +3146,10 @@
         <v>1</v>
       </c>
       <c r="BE7" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="BF7" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="BG7" s="0" t="n">
         <v>5</v>
@@ -3176,19 +3179,19 @@
         <v>14</v>
       </c>
       <c r="BP7" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BR7" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BS7" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BT7" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BU7" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BV7" s="0" t="n">
         <v>10</v>
@@ -3245,25 +3248,25 @@
         <v>3</v>
       </c>
       <c r="CN7" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="CO7" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="CP7" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="CQ7" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="CR7" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="CS7" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CT7" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="CU7" s="0" t="n">
         <v>10</v>
@@ -3299,19 +3302,19 @@
         <v>5</v>
       </c>
       <c r="DF7" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DH7" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="DI7" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="DJ7" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DK7" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="DL7" s="0" t="n">
         <v>10</v>
@@ -3338,16 +3341,16 @@
         <v>1</v>
       </c>
       <c r="DV7" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="DW7" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="DX7" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DY7" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DZ7" s="0" t="n">
         <v>100</v>
@@ -3374,15 +3377,15 @@
         <v>1</v>
       </c>
       <c r="EI7" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -3395,22 +3398,22 @@
         <v>hzb_TestP_AA_1_c-6</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>10</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M8" s="0" t="n">
         <v>100</v>
@@ -3419,7 +3422,7 @@
         <v>10</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P8" s="0" t="n">
         <v>10</v>
@@ -3428,7 +3431,7 @@
         <v>100</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S8" s="0" t="n">
         <v>20</v>
@@ -3437,22 +3440,22 @@
         <v>50</v>
       </c>
       <c r="U8" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="V8" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="W8" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="X8" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Y8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="Z8" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AA8" s="0" t="n">
         <v>2</v>
@@ -3482,7 +3485,7 @@
         <v>10</v>
       </c>
       <c r="AJ8" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AK8" s="0" t="n">
         <v>10</v>
@@ -3503,40 +3506,40 @@
         <v>100</v>
       </c>
       <c r="AQ8" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AR8" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AS8" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AT8" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AU8" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AV8" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AW8" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AX8" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AY8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AZ8" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BA8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BB8" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BC8" s="0" t="n">
         <v>10</v>
@@ -3545,10 +3548,10 @@
         <v>1</v>
       </c>
       <c r="BE8" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="BF8" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="BG8" s="0" t="n">
         <v>5</v>
@@ -3578,19 +3581,19 @@
         <v>14</v>
       </c>
       <c r="BP8" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BR8" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BS8" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BT8" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BU8" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BV8" s="0" t="n">
         <v>10</v>
@@ -3647,25 +3650,25 @@
         <v>3</v>
       </c>
       <c r="CN8" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="CO8" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="CP8" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="CQ8" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="CR8" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="CS8" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CT8" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="CU8" s="0" t="n">
         <v>10</v>
@@ -3701,19 +3704,19 @@
         <v>5</v>
       </c>
       <c r="DF8" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DH8" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="DI8" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="DJ8" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DK8" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="DL8" s="0" t="n">
         <v>10</v>
@@ -3740,16 +3743,16 @@
         <v>1</v>
       </c>
       <c r="DV8" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="DW8" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="DX8" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DY8" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DZ8" s="0" t="n">
         <v>100</v>
@@ -3776,15 +3779,15 @@
         <v>1</v>
       </c>
       <c r="EI8" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>1</v>
@@ -3797,22 +3800,22 @@
         <v>hzb_TestP_AA_1_c-7</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>10</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M9" s="0" t="n">
         <v>100</v>
@@ -3821,7 +3824,7 @@
         <v>10</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P9" s="0" t="n">
         <v>10</v>
@@ -3830,7 +3833,7 @@
         <v>100</v>
       </c>
       <c r="R9" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S9" s="0" t="n">
         <v>20</v>
@@ -3839,22 +3842,22 @@
         <v>50</v>
       </c>
       <c r="U9" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="V9" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="W9" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="X9" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Y9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="Z9" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AA9" s="0" t="n">
         <v>2</v>
@@ -3884,7 +3887,7 @@
         <v>10</v>
       </c>
       <c r="AJ9" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AK9" s="0" t="n">
         <v>10</v>
@@ -3905,40 +3908,40 @@
         <v>100</v>
       </c>
       <c r="AQ9" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AR9" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AS9" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AT9" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AU9" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AV9" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AW9" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AX9" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AY9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AZ9" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BA9" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BB9" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BC9" s="0" t="n">
         <v>10</v>
@@ -3947,10 +3950,10 @@
         <v>1</v>
       </c>
       <c r="BE9" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="BF9" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="BG9" s="0" t="n">
         <v>5</v>
@@ -3980,19 +3983,19 @@
         <v>14</v>
       </c>
       <c r="BP9" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BR9" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BS9" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BT9" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BU9" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BV9" s="0" t="n">
         <v>10</v>
@@ -4049,25 +4052,25 @@
         <v>3</v>
       </c>
       <c r="CN9" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="CO9" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="CP9" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="CQ9" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="CR9" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="CS9" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CT9" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="CU9" s="0" t="n">
         <v>10</v>
@@ -4103,19 +4106,19 @@
         <v>5</v>
       </c>
       <c r="DF9" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DH9" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="DI9" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="DJ9" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DK9" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="DL9" s="0" t="n">
         <v>10</v>
@@ -4142,16 +4145,16 @@
         <v>1</v>
       </c>
       <c r="DV9" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="DW9" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="DX9" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DY9" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DZ9" s="0" t="n">
         <v>100</v>
@@ -4178,15 +4181,15 @@
         <v>1</v>
       </c>
       <c r="EI9" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
@@ -4199,22 +4202,22 @@
         <v>hzb_TestP_AA_1_c-8</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>10</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M10" s="0" t="n">
         <v>100</v>
@@ -4223,7 +4226,7 @@
         <v>10</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P10" s="0" t="n">
         <v>10</v>
@@ -4232,7 +4235,7 @@
         <v>100</v>
       </c>
       <c r="R10" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S10" s="0" t="n">
         <v>20</v>
@@ -4241,22 +4244,22 @@
         <v>50</v>
       </c>
       <c r="U10" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="V10" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="W10" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="X10" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Y10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="Z10" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AA10" s="0" t="n">
         <v>2</v>
@@ -4286,7 +4289,7 @@
         <v>10</v>
       </c>
       <c r="AJ10" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AK10" s="0" t="n">
         <v>10</v>
@@ -4307,40 +4310,40 @@
         <v>100</v>
       </c>
       <c r="AQ10" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AR10" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AS10" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AT10" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AU10" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AV10" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AW10" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AX10" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AY10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AZ10" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BA10" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BB10" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BC10" s="0" t="n">
         <v>10</v>
@@ -4349,10 +4352,10 @@
         <v>1</v>
       </c>
       <c r="BE10" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="BF10" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="BG10" s="0" t="n">
         <v>5</v>
@@ -4382,19 +4385,19 @@
         <v>14</v>
       </c>
       <c r="BP10" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BR10" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BS10" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BT10" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BU10" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BV10" s="0" t="n">
         <v>10</v>
@@ -4451,25 +4454,25 @@
         <v>3</v>
       </c>
       <c r="CN10" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="CO10" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="CP10" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="CQ10" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="CR10" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="CS10" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CT10" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="CU10" s="0" t="n">
         <v>10</v>
@@ -4505,19 +4508,19 @@
         <v>5</v>
       </c>
       <c r="DF10" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DH10" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="DI10" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="DJ10" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DK10" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="DL10" s="0" t="n">
         <v>10</v>
@@ -4544,16 +4547,16 @@
         <v>1</v>
       </c>
       <c r="DV10" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="DW10" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="DX10" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DY10" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DZ10" s="0" t="n">
         <v>100</v>
@@ -4580,15 +4583,15 @@
         <v>1</v>
       </c>
       <c r="EI10" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>2</v>
@@ -4601,22 +4604,22 @@
         <v>hzb_TestP_AA_2_c-1</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M11" s="0" t="n">
         <v>100</v>
@@ -4625,7 +4628,7 @@
         <v>10</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P11" s="0" t="n">
         <v>10</v>
@@ -4634,7 +4637,7 @@
         <v>100</v>
       </c>
       <c r="R11" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S11" s="0" t="n">
         <v>20</v>
@@ -4643,22 +4646,22 @@
         <v>50</v>
       </c>
       <c r="U11" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="V11" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="W11" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="X11" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Y11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="Z11" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AA11" s="0" t="n">
         <v>2</v>
@@ -4688,7 +4691,7 @@
         <v>10</v>
       </c>
       <c r="AJ11" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AK11" s="0" t="n">
         <v>10</v>
@@ -4709,40 +4712,40 @@
         <v>100</v>
       </c>
       <c r="AQ11" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AR11" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AS11" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AT11" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AU11" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AV11" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AW11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AX11" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AY11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AZ11" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BA11" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BB11" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BC11" s="0" t="n">
         <v>10</v>
@@ -4751,10 +4754,10 @@
         <v>1</v>
       </c>
       <c r="BE11" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="BF11" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="BG11" s="0" t="n">
         <v>5</v>
@@ -4784,19 +4787,19 @@
         <v>14</v>
       </c>
       <c r="BP11" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BR11" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BS11" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BT11" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BU11" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BV11" s="0" t="n">
         <v>10</v>
@@ -4853,25 +4856,25 @@
         <v>3</v>
       </c>
       <c r="CN11" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="CO11" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="CP11" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="CQ11" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="CR11" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="CS11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CT11" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="CU11" s="0" t="n">
         <v>10</v>
@@ -4907,19 +4910,19 @@
         <v>5</v>
       </c>
       <c r="DF11" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DH11" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="DI11" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="DJ11" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DK11" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="DL11" s="0" t="n">
         <v>10</v>
@@ -4946,16 +4949,16 @@
         <v>1</v>
       </c>
       <c r="DV11" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="DW11" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="DX11" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DY11" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DZ11" s="0" t="n">
         <v>100</v>
@@ -4982,15 +4985,15 @@
         <v>1</v>
       </c>
       <c r="EI11" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>2</v>
@@ -5003,22 +5006,22 @@
         <v>hzb_TestP_AA_2_c-2</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>10</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M12" s="0" t="n">
         <v>100</v>
@@ -5027,7 +5030,7 @@
         <v>10</v>
       </c>
       <c r="O12" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P12" s="0" t="n">
         <v>10</v>
@@ -5036,7 +5039,7 @@
         <v>100</v>
       </c>
       <c r="R12" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S12" s="0" t="n">
         <v>20</v>
@@ -5045,22 +5048,22 @@
         <v>50</v>
       </c>
       <c r="U12" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="V12" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="W12" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="X12" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Y12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="Z12" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AA12" s="0" t="n">
         <v>2</v>
@@ -5090,7 +5093,7 @@
         <v>10</v>
       </c>
       <c r="AJ12" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AK12" s="0" t="n">
         <v>10</v>
@@ -5111,40 +5114,40 @@
         <v>100</v>
       </c>
       <c r="AQ12" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AR12" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AS12" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AT12" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AU12" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AV12" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AW12" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AX12" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AY12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AZ12" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BA12" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BB12" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BC12" s="0" t="n">
         <v>10</v>
@@ -5153,10 +5156,10 @@
         <v>1</v>
       </c>
       <c r="BE12" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="BF12" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="BG12" s="0" t="n">
         <v>5</v>
@@ -5186,19 +5189,19 @@
         <v>14</v>
       </c>
       <c r="BP12" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BR12" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BS12" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BT12" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BU12" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BV12" s="0" t="n">
         <v>10</v>
@@ -5255,25 +5258,25 @@
         <v>3</v>
       </c>
       <c r="CN12" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="CO12" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="CP12" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="CQ12" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="CR12" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="CS12" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CT12" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="CU12" s="0" t="n">
         <v>10</v>
@@ -5309,19 +5312,19 @@
         <v>5</v>
       </c>
       <c r="DF12" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DH12" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="DI12" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="DJ12" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DK12" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="DL12" s="0" t="n">
         <v>10</v>
@@ -5348,16 +5351,16 @@
         <v>1</v>
       </c>
       <c r="DV12" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="DW12" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="DX12" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DY12" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DZ12" s="0" t="n">
         <v>100</v>
@@ -5384,15 +5387,15 @@
         <v>1</v>
       </c>
       <c r="EI12" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>2</v>
@@ -5405,22 +5408,22 @@
         <v>hzb_TestP_AA_2_c-3</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>10</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M13" s="0" t="n">
         <v>100</v>
@@ -5429,7 +5432,7 @@
         <v>10</v>
       </c>
       <c r="O13" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P13" s="0" t="n">
         <v>10</v>
@@ -5438,7 +5441,7 @@
         <v>100</v>
       </c>
       <c r="R13" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S13" s="0" t="n">
         <v>20</v>
@@ -5447,22 +5450,22 @@
         <v>50</v>
       </c>
       <c r="U13" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="V13" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="W13" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="X13" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Y13" s="0" t="n">
         <v>1</v>
       </c>
       <c r="Z13" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AA13" s="0" t="n">
         <v>2</v>
@@ -5492,7 +5495,7 @@
         <v>10</v>
       </c>
       <c r="AJ13" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AK13" s="0" t="n">
         <v>10</v>
@@ -5513,40 +5516,40 @@
         <v>100</v>
       </c>
       <c r="AQ13" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AR13" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AS13" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AT13" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AU13" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AV13" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AW13" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AX13" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AY13" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AZ13" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BA13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BB13" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BC13" s="0" t="n">
         <v>10</v>
@@ -5555,10 +5558,10 @@
         <v>1</v>
       </c>
       <c r="BE13" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="BF13" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="BG13" s="0" t="n">
         <v>5</v>
@@ -5588,19 +5591,19 @@
         <v>14</v>
       </c>
       <c r="BP13" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BR13" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BS13" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BT13" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BU13" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BV13" s="0" t="n">
         <v>10</v>
@@ -5657,25 +5660,25 @@
         <v>3</v>
       </c>
       <c r="CN13" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="CO13" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="CP13" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="CQ13" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="CR13" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="CS13" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CT13" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="CU13" s="0" t="n">
         <v>10</v>
@@ -5711,19 +5714,19 @@
         <v>5</v>
       </c>
       <c r="DF13" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DH13" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="DI13" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="DJ13" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DK13" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="DL13" s="0" t="n">
         <v>10</v>
@@ -5750,16 +5753,16 @@
         <v>1</v>
       </c>
       <c r="DV13" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="DW13" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="DX13" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DY13" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DZ13" s="0" t="n">
         <v>100</v>
@@ -5786,15 +5789,15 @@
         <v>1</v>
       </c>
       <c r="EI13" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>2</v>
@@ -5807,22 +5810,22 @@
         <v>hzb_TestP_AA_2_c-4</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>10</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M14" s="0" t="n">
         <v>100</v>
@@ -5831,7 +5834,7 @@
         <v>10</v>
       </c>
       <c r="O14" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P14" s="0" t="n">
         <v>10</v>
@@ -5840,7 +5843,7 @@
         <v>100</v>
       </c>
       <c r="R14" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S14" s="0" t="n">
         <v>20</v>
@@ -5849,22 +5852,22 @@
         <v>50</v>
       </c>
       <c r="U14" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="V14" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="W14" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="X14" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Y14" s="0" t="n">
         <v>1</v>
       </c>
       <c r="Z14" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AA14" s="0" t="n">
         <v>2</v>
@@ -5894,7 +5897,7 @@
         <v>10</v>
       </c>
       <c r="AJ14" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AK14" s="0" t="n">
         <v>10</v>
@@ -5915,40 +5918,40 @@
         <v>100</v>
       </c>
       <c r="AQ14" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AR14" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AS14" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AT14" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AU14" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AV14" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AW14" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AX14" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AY14" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AZ14" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BA14" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BB14" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BC14" s="0" t="n">
         <v>10</v>
@@ -5957,10 +5960,10 @@
         <v>1</v>
       </c>
       <c r="BE14" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="BF14" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="BG14" s="0" t="n">
         <v>5</v>
@@ -5990,19 +5993,19 @@
         <v>14</v>
       </c>
       <c r="BP14" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BR14" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BS14" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BT14" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BU14" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BV14" s="0" t="n">
         <v>10</v>
@@ -6059,25 +6062,25 @@
         <v>3</v>
       </c>
       <c r="CN14" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="CO14" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="CP14" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="CQ14" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="CR14" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="CS14" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CT14" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="CU14" s="0" t="n">
         <v>10</v>
@@ -6113,19 +6116,19 @@
         <v>5</v>
       </c>
       <c r="DF14" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DH14" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="DI14" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="DJ14" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DK14" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="DL14" s="0" t="n">
         <v>10</v>
@@ -6152,16 +6155,16 @@
         <v>1</v>
       </c>
       <c r="DV14" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="DW14" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="DX14" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DY14" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DZ14" s="0" t="n">
         <v>100</v>
@@ -6188,15 +6191,15 @@
         <v>1</v>
       </c>
       <c r="EI14" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>2</v>
@@ -6209,22 +6212,22 @@
         <v>hzb_TestP_AA_2_c-5</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>10</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M15" s="0" t="n">
         <v>100</v>
@@ -6233,7 +6236,7 @@
         <v>10</v>
       </c>
       <c r="O15" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P15" s="0" t="n">
         <v>10</v>
@@ -6242,7 +6245,7 @@
         <v>100</v>
       </c>
       <c r="R15" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S15" s="0" t="n">
         <v>20</v>
@@ -6251,22 +6254,22 @@
         <v>50</v>
       </c>
       <c r="U15" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="V15" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="W15" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="X15" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Y15" s="0" t="n">
         <v>1</v>
       </c>
       <c r="Z15" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AA15" s="0" t="n">
         <v>2</v>
@@ -6296,7 +6299,7 @@
         <v>10</v>
       </c>
       <c r="AJ15" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AK15" s="0" t="n">
         <v>10</v>
@@ -6317,40 +6320,40 @@
         <v>100</v>
       </c>
       <c r="AQ15" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AR15" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AS15" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AT15" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AU15" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AV15" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AW15" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AX15" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AY15" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AZ15" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BA15" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BB15" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BC15" s="0" t="n">
         <v>10</v>
@@ -6359,10 +6362,10 @@
         <v>1</v>
       </c>
       <c r="BE15" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="BF15" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="BG15" s="0" t="n">
         <v>5</v>
@@ -6392,19 +6395,19 @@
         <v>14</v>
       </c>
       <c r="BP15" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BR15" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BS15" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BT15" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BU15" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BV15" s="0" t="n">
         <v>10</v>
@@ -6461,25 +6464,25 @@
         <v>3</v>
       </c>
       <c r="CN15" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="CO15" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="CP15" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="CQ15" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="CR15" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="CS15" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CT15" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="CU15" s="0" t="n">
         <v>10</v>
@@ -6515,19 +6518,19 @@
         <v>5</v>
       </c>
       <c r="DF15" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DH15" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="DI15" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="DJ15" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DK15" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="DL15" s="0" t="n">
         <v>10</v>
@@ -6554,16 +6557,16 @@
         <v>1</v>
       </c>
       <c r="DV15" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="DW15" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="DX15" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DY15" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DZ15" s="0" t="n">
         <v>100</v>
@@ -6590,15 +6593,15 @@
         <v>1</v>
       </c>
       <c r="EI15" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>2</v>
@@ -6611,22 +6614,22 @@
         <v>hzb_TestP_AA_2_c-6</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>10</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M16" s="0" t="n">
         <v>100</v>
@@ -6635,7 +6638,7 @@
         <v>10</v>
       </c>
       <c r="O16" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P16" s="0" t="n">
         <v>10</v>
@@ -6644,7 +6647,7 @@
         <v>100</v>
       </c>
       <c r="R16" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S16" s="0" t="n">
         <v>20</v>
@@ -6653,22 +6656,22 @@
         <v>50</v>
       </c>
       <c r="U16" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="V16" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="W16" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="X16" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Y16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="Z16" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AA16" s="0" t="n">
         <v>2</v>
@@ -6698,7 +6701,7 @@
         <v>10</v>
       </c>
       <c r="AJ16" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AK16" s="0" t="n">
         <v>10</v>
@@ -6719,40 +6722,40 @@
         <v>100</v>
       </c>
       <c r="AQ16" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AR16" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AS16" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AT16" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AU16" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AV16" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AW16" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AX16" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AY16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AZ16" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BA16" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BB16" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BC16" s="0" t="n">
         <v>10</v>
@@ -6761,10 +6764,10 @@
         <v>1</v>
       </c>
       <c r="BE16" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="BF16" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="BG16" s="0" t="n">
         <v>5</v>
@@ -6794,19 +6797,19 @@
         <v>14</v>
       </c>
       <c r="BP16" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BR16" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BS16" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BT16" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BU16" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BV16" s="0" t="n">
         <v>10</v>
@@ -6863,25 +6866,25 @@
         <v>3</v>
       </c>
       <c r="CN16" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="CO16" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="CP16" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="CQ16" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="CR16" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="CS16" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CT16" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="CU16" s="0" t="n">
         <v>10</v>
@@ -6917,19 +6920,19 @@
         <v>5</v>
       </c>
       <c r="DF16" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DH16" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="DI16" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="DJ16" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DK16" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="DL16" s="0" t="n">
         <v>10</v>
@@ -6956,16 +6959,16 @@
         <v>1</v>
       </c>
       <c r="DV16" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="DW16" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="DX16" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DY16" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DZ16" s="0" t="n">
         <v>100</v>
@@ -6992,15 +6995,15 @@
         <v>1</v>
       </c>
       <c r="EI16" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>2</v>
@@ -7013,22 +7016,22 @@
         <v>hzb_TestP_AA_2_c-7</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>10</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M17" s="0" t="n">
         <v>100</v>
@@ -7037,7 +7040,7 @@
         <v>10</v>
       </c>
       <c r="O17" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P17" s="0" t="n">
         <v>10</v>
@@ -7046,7 +7049,7 @@
         <v>100</v>
       </c>
       <c r="R17" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S17" s="0" t="n">
         <v>20</v>
@@ -7055,22 +7058,22 @@
         <v>50</v>
       </c>
       <c r="U17" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="V17" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="W17" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="X17" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Y17" s="0" t="n">
         <v>1</v>
       </c>
       <c r="Z17" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AA17" s="0" t="n">
         <v>2</v>
@@ -7100,7 +7103,7 @@
         <v>10</v>
       </c>
       <c r="AJ17" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AK17" s="0" t="n">
         <v>10</v>
@@ -7121,40 +7124,40 @@
         <v>100</v>
       </c>
       <c r="AQ17" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AR17" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AS17" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AT17" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AU17" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AV17" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AW17" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AX17" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AY17" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AZ17" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BA17" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BB17" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BC17" s="0" t="n">
         <v>10</v>
@@ -7163,10 +7166,10 @@
         <v>1</v>
       </c>
       <c r="BE17" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="BF17" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="BG17" s="0" t="n">
         <v>5</v>
@@ -7196,19 +7199,19 @@
         <v>14</v>
       </c>
       <c r="BP17" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BR17" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BS17" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BT17" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BU17" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BV17" s="0" t="n">
         <v>10</v>
@@ -7265,25 +7268,25 @@
         <v>3</v>
       </c>
       <c r="CN17" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="CO17" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="CP17" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="CQ17" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="CR17" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="CS17" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CT17" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="CU17" s="0" t="n">
         <v>10</v>
@@ -7319,19 +7322,19 @@
         <v>5</v>
       </c>
       <c r="DF17" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DH17" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="DI17" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="DJ17" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DK17" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="DL17" s="0" t="n">
         <v>10</v>
@@ -7358,16 +7361,16 @@
         <v>1</v>
       </c>
       <c r="DV17" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="DW17" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="DX17" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DY17" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DZ17" s="0" t="n">
         <v>100</v>
@@ -7394,15 +7397,15 @@
         <v>1</v>
       </c>
       <c r="EI17" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>2</v>
@@ -7415,22 +7418,22 @@
         <v>hzb_TestP_AA_2_c-8</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>10</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M18" s="0" t="n">
         <v>100</v>
@@ -7439,7 +7442,7 @@
         <v>10</v>
       </c>
       <c r="O18" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P18" s="0" t="n">
         <v>10</v>
@@ -7448,7 +7451,7 @@
         <v>100</v>
       </c>
       <c r="R18" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S18" s="0" t="n">
         <v>20</v>
@@ -7457,22 +7460,22 @@
         <v>50</v>
       </c>
       <c r="U18" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="V18" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="W18" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="X18" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Y18" s="0" t="n">
         <v>1</v>
       </c>
       <c r="Z18" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AA18" s="0" t="n">
         <v>2</v>
@@ -7502,7 +7505,7 @@
         <v>10</v>
       </c>
       <c r="AJ18" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AK18" s="0" t="n">
         <v>10</v>
@@ -7523,40 +7526,40 @@
         <v>100</v>
       </c>
       <c r="AQ18" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AR18" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AS18" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AT18" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AU18" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AV18" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AW18" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AX18" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AY18" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AZ18" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BA18" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BB18" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BC18" s="0" t="n">
         <v>10</v>
@@ -7565,10 +7568,10 @@
         <v>1</v>
       </c>
       <c r="BE18" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="BF18" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="BG18" s="0" t="n">
         <v>5</v>
@@ -7598,19 +7601,19 @@
         <v>14</v>
       </c>
       <c r="BP18" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BR18" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BS18" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BT18" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BU18" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BV18" s="0" t="n">
         <v>10</v>
@@ -7667,25 +7670,25 @@
         <v>3</v>
       </c>
       <c r="CN18" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="CO18" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="CP18" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="CQ18" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="CR18" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="CS18" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CT18" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="CU18" s="0" t="n">
         <v>10</v>
@@ -7721,19 +7724,19 @@
         <v>5</v>
       </c>
       <c r="DF18" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DH18" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="DI18" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="DJ18" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DK18" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="DL18" s="0" t="n">
         <v>10</v>
@@ -7760,16 +7763,16 @@
         <v>1</v>
       </c>
       <c r="DV18" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="DW18" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="DX18" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="DY18" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="DZ18" s="0" t="n">
         <v>100</v>
@@ -7796,7 +7799,7 @@
         <v>1</v>
       </c>
       <c r="EI18" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
updated test for concetration
</commit_message>
<xml_diff>
--- a/tests/data/20250114_experiment_file.xlsx
+++ b/tests/data/20250114_experiment_file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="155">
   <si>
     <t xml:space="preserve">Experiment Info</t>
   </si>
@@ -145,61 +145,64 @@
     <t xml:space="preserve">Solute 1 name</t>
   </si>
   <si>
+    <t xml:space="preserve">Solute 1 Concentration [mg/ml]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solute 1 relative amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solution volume [um]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spin Delay [s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotation speed 1 [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotation time 1 [s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acceleration 1 [rpm/s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotation speed 2 [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotation time 2 [s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acceleration 2 [rpm/s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anti solvent name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anti solvent volume [ml]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anti solvent dropping time [s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anti solvent dropping speed [ul/s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anti solvent dropping heigt [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annealing time [min]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annealing temperature [°C]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annealing athmosphere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solute 1 type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Solute 1 Concentration [mM]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solute 1 relative amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solution volume [um]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spin Delay [s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rotation speed 1 [rpm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rotation time 1 [s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acceleration 1 [rpm/s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rotation speed 2 [rpm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rotation time 2 [s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acceleration 2 [rpm/s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anti solvent name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anti solvent volume [ml]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anti solvent dropping time [s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anti solvent dropping speed [ul/s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anti solvent dropping heigt [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annealing time [min]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annealing temperature [°C]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annealing athmosphere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solute 1 type</t>
   </si>
   <si>
     <t xml:space="preserve">Solute 2 type</t>
@@ -661,8 +664,8 @@
   </sheetPr>
   <dimension ref="A1:EP18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2:K18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AF2" activeCellId="0" sqref="AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1142,49 +1145,49 @@
         <v>59</v>
       </c>
       <c r="BE2" s="2" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="BF2" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="BG2" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="BH2" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="BI2" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="BJ2" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="BK2" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="BL2" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="BM2" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="BN2" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BO2" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="BP2" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="BQ2" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="BR2" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="BS2" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="BT2" s="2" t="s">
         <v>56</v>
@@ -1208,64 +1211,64 @@
         <v>36</v>
       </c>
       <c r="CA2" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="CB2" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="CC2" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="CD2" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="CE2" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="CF2" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="CG2" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="CH2" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="CI2" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="CJ2" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="CK2" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="CL2" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="CM2" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="CN2" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="CO2" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="CP2" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="CQ2" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="CR2" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="CS2" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="CT2" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="CU2" s="2" t="s">
         <v>34</v>
@@ -1286,31 +1289,31 @@
         <v>59</v>
       </c>
       <c r="DA2" s="2" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="DB2" s="2" t="s">
         <v>43</v>
       </c>
       <c r="DC2" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="DD2" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="DE2" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="DF2" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="DG2" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="DH2" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="DI2" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="DJ2" s="2" t="s">
         <v>56</v>
@@ -1334,34 +1337,34 @@
         <v>36</v>
       </c>
       <c r="DQ2" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="DR2" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="DS2" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="DT2" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="DU2" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="DV2" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="DW2" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="DX2" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="DY2" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="DZ2" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="EA2" s="2" t="s">
         <v>20</v>
@@ -1376,37 +1379,37 @@
         <v>36</v>
       </c>
       <c r="EE2" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="EF2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="EG2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="EH2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="EI2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="EJ2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="EK2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="EL2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="EG2" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="EH2" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="EI2" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="EJ2" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="EK2" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="EL2" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="EM2" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="EN2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="EO2" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="EP2" s="2" t="s">
         <v>20</v>
@@ -1414,10 +1417,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
@@ -1430,7 +1433,7 @@
         <v>hzb_TestP_AA_1_c-1</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>0.16</v>
@@ -1442,22 +1445,22 @@
         <v>1</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M3" s="0" t="n">
         <v>10</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q3" s="0" t="n">
         <v>100</v>
@@ -1466,7 +1469,7 @@
         <v>10</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="T3" s="0" t="n">
         <v>10</v>
@@ -1475,7 +1478,7 @@
         <v>100</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="W3" s="0" t="n">
         <v>20</v>
@@ -1484,16 +1487,16 @@
         <v>50</v>
       </c>
       <c r="Y3" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA3" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AB3" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AC3" s="0" t="n">
         <v>1</v>
@@ -1502,7 +1505,7 @@
         <v>1</v>
       </c>
       <c r="AE3" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AF3" s="0" t="n">
         <v>2</v>
@@ -1535,7 +1538,7 @@
         <v>10</v>
       </c>
       <c r="AP3" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AQ3" s="0" t="n">
         <v>10</v>
@@ -1556,40 +1559,40 @@
         <v>100</v>
       </c>
       <c r="AW3" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AX3" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AY3" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AZ3" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BA3" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BB3" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BC3" s="0" t="n">
         <v>10</v>
       </c>
       <c r="BD3" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BE3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="BF3" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BG3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BH3" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="BI3" s="0" t="n">
         <v>10</v>
@@ -1598,10 +1601,10 @@
         <v>1</v>
       </c>
       <c r="BK3" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL3" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BM3" s="0" t="n">
         <v>5</v>
@@ -1631,19 +1634,19 @@
         <v>14</v>
       </c>
       <c r="BV3" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="BX3" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BY3" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="BZ3" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="CA3" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="CB3" s="0" t="n">
         <v>10</v>
@@ -1700,25 +1703,25 @@
         <v>3</v>
       </c>
       <c r="CT3" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="CU3" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="CV3" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="CW3" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="CX3" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="CY3" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CZ3" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="DA3" s="0" t="n">
         <v>10</v>
@@ -1754,19 +1757,19 @@
         <v>5</v>
       </c>
       <c r="DL3" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="DN3" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="DO3" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="DP3" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="DQ3" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="DR3" s="0" t="n">
         <v>10</v>
@@ -1793,16 +1796,16 @@
         <v>1</v>
       </c>
       <c r="EB3" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="EC3" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="ED3" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="EE3" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="EF3" s="0" t="n">
         <v>100</v>
@@ -1829,15 +1832,15 @@
         <v>1</v>
       </c>
       <c r="EO3" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -1850,7 +1853,7 @@
         <v>hzb_TestP_AA_1_c-2</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>0.16</v>
@@ -1862,22 +1865,22 @@
         <v>1</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M4" s="0" t="n">
         <v>10</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q4" s="0" t="n">
         <v>100</v>
@@ -1886,7 +1889,7 @@
         <v>10</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="T4" s="0" t="n">
         <v>10</v>
@@ -1895,7 +1898,7 @@
         <v>100</v>
       </c>
       <c r="V4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="W4" s="0" t="n">
         <v>20</v>
@@ -1904,16 +1907,16 @@
         <v>50</v>
       </c>
       <c r="Y4" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Z4" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA4" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AB4" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AC4" s="0" t="n">
         <v>1</v>
@@ -1922,7 +1925,7 @@
         <v>1</v>
       </c>
       <c r="AE4" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AF4" s="0" t="n">
         <v>2</v>
@@ -1955,7 +1958,7 @@
         <v>10</v>
       </c>
       <c r="AP4" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AQ4" s="0" t="n">
         <v>10</v>
@@ -1976,40 +1979,40 @@
         <v>100</v>
       </c>
       <c r="AW4" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AX4" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AY4" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AZ4" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BA4" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BB4" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BC4" s="0" t="n">
         <v>10</v>
       </c>
       <c r="BD4" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BE4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="BF4" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BG4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BH4" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="BI4" s="0" t="n">
         <v>10</v>
@@ -2018,10 +2021,10 @@
         <v>1</v>
       </c>
       <c r="BK4" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL4" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BM4" s="0" t="n">
         <v>5</v>
@@ -2051,19 +2054,19 @@
         <v>14</v>
       </c>
       <c r="BV4" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="BX4" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BY4" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="BZ4" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="CA4" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="CB4" s="0" t="n">
         <v>10</v>
@@ -2120,25 +2123,25 @@
         <v>3</v>
       </c>
       <c r="CT4" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="CU4" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="CV4" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="CW4" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="CX4" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="CY4" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CZ4" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="DA4" s="0" t="n">
         <v>10</v>
@@ -2174,19 +2177,19 @@
         <v>5</v>
       </c>
       <c r="DL4" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="DN4" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="DO4" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="DP4" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="DQ4" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="DR4" s="0" t="n">
         <v>10</v>
@@ -2213,16 +2216,16 @@
         <v>1</v>
       </c>
       <c r="EB4" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="EC4" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="ED4" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="EE4" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="EF4" s="0" t="n">
         <v>100</v>
@@ -2249,15 +2252,15 @@
         <v>1</v>
       </c>
       <c r="EO4" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
@@ -2270,7 +2273,7 @@
         <v>hzb_TestP_AA_1_c-3</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>0.16</v>
@@ -2282,22 +2285,22 @@
         <v>1</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M5" s="0" t="n">
         <v>10</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q5" s="0" t="n">
         <v>100</v>
@@ -2306,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="T5" s="0" t="n">
         <v>10</v>
@@ -2315,7 +2318,7 @@
         <v>100</v>
       </c>
       <c r="V5" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="W5" s="0" t="n">
         <v>20</v>
@@ -2324,16 +2327,16 @@
         <v>50</v>
       </c>
       <c r="Y5" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Z5" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA5" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AB5" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AC5" s="0" t="n">
         <v>1</v>
@@ -2342,7 +2345,7 @@
         <v>1</v>
       </c>
       <c r="AE5" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AF5" s="0" t="n">
         <v>2</v>
@@ -2375,7 +2378,7 @@
         <v>10</v>
       </c>
       <c r="AP5" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AQ5" s="0" t="n">
         <v>10</v>
@@ -2396,40 +2399,40 @@
         <v>100</v>
       </c>
       <c r="AW5" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AX5" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AY5" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AZ5" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BA5" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BB5" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BC5" s="0" t="n">
         <v>10</v>
       </c>
       <c r="BD5" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BE5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="BF5" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BG5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BH5" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="BI5" s="0" t="n">
         <v>10</v>
@@ -2438,10 +2441,10 @@
         <v>1</v>
       </c>
       <c r="BK5" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL5" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BM5" s="0" t="n">
         <v>5</v>
@@ -2471,19 +2474,19 @@
         <v>14</v>
       </c>
       <c r="BV5" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="BX5" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BY5" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="BZ5" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="CA5" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="CB5" s="0" t="n">
         <v>10</v>
@@ -2540,25 +2543,25 @@
         <v>3</v>
       </c>
       <c r="CT5" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="CU5" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="CV5" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="CW5" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="CX5" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="CY5" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CZ5" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="DA5" s="0" t="n">
         <v>10</v>
@@ -2594,19 +2597,19 @@
         <v>5</v>
       </c>
       <c r="DL5" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="DN5" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="DO5" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="DP5" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="DQ5" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="DR5" s="0" t="n">
         <v>10</v>
@@ -2633,16 +2636,16 @@
         <v>1</v>
       </c>
       <c r="EB5" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="EC5" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="ED5" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="EE5" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="EF5" s="0" t="n">
         <v>100</v>
@@ -2669,15 +2672,15 @@
         <v>1</v>
       </c>
       <c r="EO5" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
@@ -2690,7 +2693,7 @@
         <v>hzb_TestP_AA_1_c-4</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>0.16</v>
@@ -2702,22 +2705,22 @@
         <v>1</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M6" s="0" t="n">
         <v>10</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q6" s="0" t="n">
         <v>100</v>
@@ -2726,7 +2729,7 @@
         <v>10</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="T6" s="0" t="n">
         <v>10</v>
@@ -2735,7 +2738,7 @@
         <v>100</v>
       </c>
       <c r="V6" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="W6" s="0" t="n">
         <v>20</v>
@@ -2744,16 +2747,16 @@
         <v>50</v>
       </c>
       <c r="Y6" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Z6" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA6" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AB6" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AC6" s="0" t="n">
         <v>1</v>
@@ -2762,7 +2765,7 @@
         <v>1</v>
       </c>
       <c r="AE6" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AF6" s="0" t="n">
         <v>2</v>
@@ -2795,7 +2798,7 @@
         <v>10</v>
       </c>
       <c r="AP6" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AQ6" s="0" t="n">
         <v>10</v>
@@ -2816,40 +2819,40 @@
         <v>100</v>
       </c>
       <c r="AW6" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AX6" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AY6" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AZ6" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BA6" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BB6" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BC6" s="0" t="n">
         <v>10</v>
       </c>
       <c r="BD6" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BE6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="BF6" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BG6" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BH6" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="BI6" s="0" t="n">
         <v>10</v>
@@ -2858,10 +2861,10 @@
         <v>1</v>
       </c>
       <c r="BK6" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL6" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BM6" s="0" t="n">
         <v>5</v>
@@ -2891,19 +2894,19 @@
         <v>14</v>
       </c>
       <c r="BV6" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="BX6" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BY6" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="BZ6" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="CA6" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="CB6" s="0" t="n">
         <v>10</v>
@@ -2960,25 +2963,25 @@
         <v>3</v>
       </c>
       <c r="CT6" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="CU6" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="CV6" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="CW6" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="CX6" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="CY6" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CZ6" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="DA6" s="0" t="n">
         <v>10</v>
@@ -3014,19 +3017,19 @@
         <v>5</v>
       </c>
       <c r="DL6" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="DN6" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="DO6" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="DP6" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="DQ6" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="DR6" s="0" t="n">
         <v>10</v>
@@ -3053,16 +3056,16 @@
         <v>1</v>
       </c>
       <c r="EB6" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="EC6" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="ED6" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="EE6" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="EF6" s="0" t="n">
         <v>100</v>
@@ -3089,15 +3092,15 @@
         <v>1</v>
       </c>
       <c r="EO6" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>1</v>
@@ -3110,7 +3113,7 @@
         <v>hzb_TestP_AA_1_c-5</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>0.16</v>
@@ -3122,22 +3125,22 @@
         <v>1</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M7" s="0" t="n">
         <v>10</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q7" s="0" t="n">
         <v>100</v>
@@ -3146,7 +3149,7 @@
         <v>10</v>
       </c>
       <c r="S7" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="T7" s="0" t="n">
         <v>10</v>
@@ -3155,7 +3158,7 @@
         <v>100</v>
       </c>
       <c r="V7" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="W7" s="0" t="n">
         <v>20</v>
@@ -3164,16 +3167,16 @@
         <v>50</v>
       </c>
       <c r="Y7" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Z7" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA7" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AB7" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AC7" s="0" t="n">
         <v>1</v>
@@ -3182,7 +3185,7 @@
         <v>1</v>
       </c>
       <c r="AE7" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AF7" s="0" t="n">
         <v>2</v>
@@ -3215,7 +3218,7 @@
         <v>10</v>
       </c>
       <c r="AP7" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AQ7" s="0" t="n">
         <v>10</v>
@@ -3236,40 +3239,40 @@
         <v>100</v>
       </c>
       <c r="AW7" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AX7" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AY7" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AZ7" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BA7" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BB7" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BC7" s="0" t="n">
         <v>10</v>
       </c>
       <c r="BD7" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BE7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="BF7" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BG7" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BH7" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="BI7" s="0" t="n">
         <v>10</v>
@@ -3278,10 +3281,10 @@
         <v>1</v>
       </c>
       <c r="BK7" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL7" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BM7" s="0" t="n">
         <v>5</v>
@@ -3311,19 +3314,19 @@
         <v>14</v>
       </c>
       <c r="BV7" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="BX7" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BY7" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="BZ7" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="CA7" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="CB7" s="0" t="n">
         <v>10</v>
@@ -3380,25 +3383,25 @@
         <v>3</v>
       </c>
       <c r="CT7" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="CU7" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="CV7" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="CW7" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="CX7" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="CY7" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CZ7" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="DA7" s="0" t="n">
         <v>10</v>
@@ -3434,19 +3437,19 @@
         <v>5</v>
       </c>
       <c r="DL7" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="DN7" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="DO7" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="DP7" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="DQ7" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="DR7" s="0" t="n">
         <v>10</v>
@@ -3473,16 +3476,16 @@
         <v>1</v>
       </c>
       <c r="EB7" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="EC7" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="ED7" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="EE7" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="EF7" s="0" t="n">
         <v>100</v>
@@ -3509,15 +3512,15 @@
         <v>1</v>
       </c>
       <c r="EO7" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -3530,7 +3533,7 @@
         <v>hzb_TestP_AA_1_c-6</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>0.16</v>
@@ -3542,22 +3545,22 @@
         <v>1</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M8" s="0" t="n">
         <v>10</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q8" s="0" t="n">
         <v>100</v>
@@ -3566,7 +3569,7 @@
         <v>10</v>
       </c>
       <c r="S8" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="T8" s="0" t="n">
         <v>10</v>
@@ -3575,7 +3578,7 @@
         <v>100</v>
       </c>
       <c r="V8" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="W8" s="0" t="n">
         <v>20</v>
@@ -3584,16 +3587,16 @@
         <v>50</v>
       </c>
       <c r="Y8" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Z8" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA8" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AB8" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AC8" s="0" t="n">
         <v>1</v>
@@ -3602,7 +3605,7 @@
         <v>1</v>
       </c>
       <c r="AE8" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AF8" s="0" t="n">
         <v>2</v>
@@ -3635,7 +3638,7 @@
         <v>10</v>
       </c>
       <c r="AP8" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AQ8" s="0" t="n">
         <v>10</v>
@@ -3656,40 +3659,40 @@
         <v>100</v>
       </c>
       <c r="AW8" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AX8" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AY8" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AZ8" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BA8" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BB8" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BC8" s="0" t="n">
         <v>10</v>
       </c>
       <c r="BD8" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BE8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="BF8" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BG8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BH8" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="BI8" s="0" t="n">
         <v>10</v>
@@ -3698,10 +3701,10 @@
         <v>1</v>
       </c>
       <c r="BK8" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL8" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BM8" s="0" t="n">
         <v>5</v>
@@ -3731,19 +3734,19 @@
         <v>14</v>
       </c>
       <c r="BV8" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="BX8" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BY8" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="BZ8" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="CA8" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="CB8" s="0" t="n">
         <v>10</v>
@@ -3800,25 +3803,25 @@
         <v>3</v>
       </c>
       <c r="CT8" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="CU8" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="CV8" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="CW8" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="CX8" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="CY8" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CZ8" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="DA8" s="0" t="n">
         <v>10</v>
@@ -3854,19 +3857,19 @@
         <v>5</v>
       </c>
       <c r="DL8" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="DN8" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="DO8" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="DP8" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="DQ8" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="DR8" s="0" t="n">
         <v>10</v>
@@ -3893,16 +3896,16 @@
         <v>1</v>
       </c>
       <c r="EB8" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="EC8" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="ED8" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="EE8" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="EF8" s="0" t="n">
         <v>100</v>
@@ -3929,15 +3932,15 @@
         <v>1</v>
       </c>
       <c r="EO8" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>1</v>
@@ -3950,7 +3953,7 @@
         <v>hzb_TestP_AA_1_c-7</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>0.16</v>
@@ -3962,22 +3965,22 @@
         <v>1</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M9" s="0" t="n">
         <v>10</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P9" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q9" s="0" t="n">
         <v>100</v>
@@ -3986,7 +3989,7 @@
         <v>10</v>
       </c>
       <c r="S9" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="T9" s="0" t="n">
         <v>10</v>
@@ -3995,7 +3998,7 @@
         <v>100</v>
       </c>
       <c r="V9" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="W9" s="0" t="n">
         <v>20</v>
@@ -4004,16 +4007,16 @@
         <v>50</v>
       </c>
       <c r="Y9" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Z9" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA9" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AB9" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AC9" s="0" t="n">
         <v>1</v>
@@ -4022,7 +4025,7 @@
         <v>1</v>
       </c>
       <c r="AE9" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AF9" s="0" t="n">
         <v>2</v>
@@ -4055,7 +4058,7 @@
         <v>10</v>
       </c>
       <c r="AP9" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AQ9" s="0" t="n">
         <v>10</v>
@@ -4076,40 +4079,40 @@
         <v>100</v>
       </c>
       <c r="AW9" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AX9" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AY9" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AZ9" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BA9" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BB9" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BC9" s="0" t="n">
         <v>10</v>
       </c>
       <c r="BD9" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BE9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="BF9" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BG9" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BH9" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="BI9" s="0" t="n">
         <v>10</v>
@@ -4118,10 +4121,10 @@
         <v>1</v>
       </c>
       <c r="BK9" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL9" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BM9" s="0" t="n">
         <v>5</v>
@@ -4151,19 +4154,19 @@
         <v>14</v>
       </c>
       <c r="BV9" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="BX9" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BY9" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="BZ9" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="CA9" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="CB9" s="0" t="n">
         <v>10</v>
@@ -4220,25 +4223,25 @@
         <v>3</v>
       </c>
       <c r="CT9" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="CU9" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="CV9" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="CW9" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="CX9" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="CY9" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CZ9" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="DA9" s="0" t="n">
         <v>10</v>
@@ -4274,19 +4277,19 @@
         <v>5</v>
       </c>
       <c r="DL9" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="DN9" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="DO9" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="DP9" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="DQ9" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="DR9" s="0" t="n">
         <v>10</v>
@@ -4313,16 +4316,16 @@
         <v>1</v>
       </c>
       <c r="EB9" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="EC9" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="ED9" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="EE9" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="EF9" s="0" t="n">
         <v>100</v>
@@ -4349,15 +4352,15 @@
         <v>1</v>
       </c>
       <c r="EO9" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
@@ -4370,7 +4373,7 @@
         <v>hzb_TestP_AA_1_c-8</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>0.16</v>
@@ -4382,22 +4385,22 @@
         <v>1</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M10" s="0" t="n">
         <v>10</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q10" s="0" t="n">
         <v>100</v>
@@ -4406,7 +4409,7 @@
         <v>10</v>
       </c>
       <c r="S10" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="T10" s="0" t="n">
         <v>10</v>
@@ -4415,7 +4418,7 @@
         <v>100</v>
       </c>
       <c r="V10" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="W10" s="0" t="n">
         <v>20</v>
@@ -4424,16 +4427,16 @@
         <v>50</v>
       </c>
       <c r="Y10" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Z10" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA10" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AB10" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AC10" s="0" t="n">
         <v>1</v>
@@ -4442,7 +4445,7 @@
         <v>1</v>
       </c>
       <c r="AE10" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AF10" s="0" t="n">
         <v>2</v>
@@ -4475,7 +4478,7 @@
         <v>10</v>
       </c>
       <c r="AP10" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AQ10" s="0" t="n">
         <v>10</v>
@@ -4496,40 +4499,40 @@
         <v>100</v>
       </c>
       <c r="AW10" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AX10" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AY10" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AZ10" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BA10" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BB10" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BC10" s="0" t="n">
         <v>10</v>
       </c>
       <c r="BD10" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BE10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="BF10" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BG10" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BH10" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="BI10" s="0" t="n">
         <v>10</v>
@@ -4538,10 +4541,10 @@
         <v>1</v>
       </c>
       <c r="BK10" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL10" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BM10" s="0" t="n">
         <v>5</v>
@@ -4571,19 +4574,19 @@
         <v>14</v>
       </c>
       <c r="BV10" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="BX10" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BY10" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="BZ10" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="CA10" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="CB10" s="0" t="n">
         <v>10</v>
@@ -4640,25 +4643,25 @@
         <v>3</v>
       </c>
       <c r="CT10" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="CU10" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="CV10" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="CW10" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="CX10" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="CY10" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CZ10" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="DA10" s="0" t="n">
         <v>10</v>
@@ -4694,19 +4697,19 @@
         <v>5</v>
       </c>
       <c r="DL10" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="DN10" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="DO10" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="DP10" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="DQ10" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="DR10" s="0" t="n">
         <v>10</v>
@@ -4733,16 +4736,16 @@
         <v>1</v>
       </c>
       <c r="EB10" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="EC10" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="ED10" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="EE10" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="EF10" s="0" t="n">
         <v>100</v>
@@ -4769,15 +4772,15 @@
         <v>1</v>
       </c>
       <c r="EO10" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>2</v>
@@ -4790,7 +4793,7 @@
         <v>hzb_TestP_AA_2_c-1</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>0.16</v>
@@ -4802,22 +4805,22 @@
         <v>1</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q11" s="0" t="n">
         <v>100</v>
@@ -4826,7 +4829,7 @@
         <v>10</v>
       </c>
       <c r="S11" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="T11" s="0" t="n">
         <v>10</v>
@@ -4835,7 +4838,7 @@
         <v>100</v>
       </c>
       <c r="V11" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="W11" s="0" t="n">
         <v>20</v>
@@ -4844,16 +4847,16 @@
         <v>50</v>
       </c>
       <c r="Y11" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Z11" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA11" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AB11" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AC11" s="0" t="n">
         <v>1</v>
@@ -4862,7 +4865,7 @@
         <v>1</v>
       </c>
       <c r="AE11" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AF11" s="0" t="n">
         <v>2</v>
@@ -4895,7 +4898,7 @@
         <v>10</v>
       </c>
       <c r="AP11" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AQ11" s="0" t="n">
         <v>10</v>
@@ -4916,40 +4919,40 @@
         <v>100</v>
       </c>
       <c r="AW11" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AX11" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AY11" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AZ11" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BA11" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BB11" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BC11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="BD11" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BE11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="BF11" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BG11" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BH11" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="BI11" s="0" t="n">
         <v>10</v>
@@ -4958,10 +4961,10 @@
         <v>1</v>
       </c>
       <c r="BK11" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL11" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BM11" s="0" t="n">
         <v>5</v>
@@ -4991,19 +4994,19 @@
         <v>14</v>
       </c>
       <c r="BV11" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="BX11" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BY11" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="BZ11" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="CA11" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="CB11" s="0" t="n">
         <v>10</v>
@@ -5060,25 +5063,25 @@
         <v>3</v>
       </c>
       <c r="CT11" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="CU11" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="CV11" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="CW11" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="CX11" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="CY11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CZ11" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="DA11" s="0" t="n">
         <v>10</v>
@@ -5114,19 +5117,19 @@
         <v>5</v>
       </c>
       <c r="DL11" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="DN11" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="DO11" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="DP11" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="DQ11" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="DR11" s="0" t="n">
         <v>10</v>
@@ -5153,16 +5156,16 @@
         <v>1</v>
       </c>
       <c r="EB11" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="EC11" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="ED11" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="EE11" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="EF11" s="0" t="n">
         <v>100</v>
@@ -5189,15 +5192,15 @@
         <v>1</v>
       </c>
       <c r="EO11" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>2</v>
@@ -5210,7 +5213,7 @@
         <v>hzb_TestP_AA_2_c-2</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>0.16</v>
@@ -5222,22 +5225,22 @@
         <v>1</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M12" s="0" t="n">
         <v>10</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O12" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P12" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q12" s="0" t="n">
         <v>100</v>
@@ -5246,7 +5249,7 @@
         <v>10</v>
       </c>
       <c r="S12" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="T12" s="0" t="n">
         <v>10</v>
@@ -5255,7 +5258,7 @@
         <v>100</v>
       </c>
       <c r="V12" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="W12" s="0" t="n">
         <v>20</v>
@@ -5264,16 +5267,16 @@
         <v>50</v>
       </c>
       <c r="Y12" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Z12" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA12" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AB12" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AC12" s="0" t="n">
         <v>1</v>
@@ -5282,7 +5285,7 @@
         <v>1</v>
       </c>
       <c r="AE12" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AF12" s="0" t="n">
         <v>2</v>
@@ -5315,7 +5318,7 @@
         <v>10</v>
       </c>
       <c r="AP12" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AQ12" s="0" t="n">
         <v>10</v>
@@ -5336,40 +5339,40 @@
         <v>100</v>
       </c>
       <c r="AW12" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AX12" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AY12" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AZ12" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BA12" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BB12" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BC12" s="0" t="n">
         <v>10</v>
       </c>
       <c r="BD12" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BE12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="BF12" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BG12" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BH12" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="BI12" s="0" t="n">
         <v>10</v>
@@ -5378,10 +5381,10 @@
         <v>1</v>
       </c>
       <c r="BK12" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL12" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BM12" s="0" t="n">
         <v>5</v>
@@ -5411,19 +5414,19 @@
         <v>14</v>
       </c>
       <c r="BV12" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="BX12" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BY12" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="BZ12" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="CA12" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="CB12" s="0" t="n">
         <v>10</v>
@@ -5480,25 +5483,25 @@
         <v>3</v>
       </c>
       <c r="CT12" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="CU12" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="CV12" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="CW12" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="CX12" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="CY12" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CZ12" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="DA12" s="0" t="n">
         <v>10</v>
@@ -5534,19 +5537,19 @@
         <v>5</v>
       </c>
       <c r="DL12" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="DN12" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="DO12" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="DP12" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="DQ12" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="DR12" s="0" t="n">
         <v>10</v>
@@ -5573,16 +5576,16 @@
         <v>1</v>
       </c>
       <c r="EB12" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="EC12" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="ED12" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="EE12" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="EF12" s="0" t="n">
         <v>100</v>
@@ -5609,15 +5612,15 @@
         <v>1</v>
       </c>
       <c r="EO12" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>2</v>
@@ -5630,7 +5633,7 @@
         <v>hzb_TestP_AA_2_c-3</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>0.16</v>
@@ -5642,22 +5645,22 @@
         <v>1</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M13" s="0" t="n">
         <v>10</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O13" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P13" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q13" s="0" t="n">
         <v>100</v>
@@ -5666,7 +5669,7 @@
         <v>10</v>
       </c>
       <c r="S13" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="T13" s="0" t="n">
         <v>10</v>
@@ -5675,7 +5678,7 @@
         <v>100</v>
       </c>
       <c r="V13" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="W13" s="0" t="n">
         <v>20</v>
@@ -5684,16 +5687,16 @@
         <v>50</v>
       </c>
       <c r="Y13" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Z13" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA13" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AB13" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AC13" s="0" t="n">
         <v>1</v>
@@ -5702,7 +5705,7 @@
         <v>1</v>
       </c>
       <c r="AE13" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AF13" s="0" t="n">
         <v>2</v>
@@ -5735,7 +5738,7 @@
         <v>10</v>
       </c>
       <c r="AP13" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AQ13" s="0" t="n">
         <v>10</v>
@@ -5756,40 +5759,40 @@
         <v>100</v>
       </c>
       <c r="AW13" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AX13" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AY13" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AZ13" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BA13" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BB13" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BC13" s="0" t="n">
         <v>10</v>
       </c>
       <c r="BD13" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BE13" s="0" t="n">
         <v>1</v>
       </c>
       <c r="BF13" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BG13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BH13" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="BI13" s="0" t="n">
         <v>10</v>
@@ -5798,10 +5801,10 @@
         <v>1</v>
       </c>
       <c r="BK13" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL13" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BM13" s="0" t="n">
         <v>5</v>
@@ -5831,19 +5834,19 @@
         <v>14</v>
       </c>
       <c r="BV13" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="BX13" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BY13" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="BZ13" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="CA13" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="CB13" s="0" t="n">
         <v>10</v>
@@ -5900,25 +5903,25 @@
         <v>3</v>
       </c>
       <c r="CT13" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="CU13" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="CV13" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="CW13" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="CX13" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="CY13" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CZ13" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="DA13" s="0" t="n">
         <v>10</v>
@@ -5954,19 +5957,19 @@
         <v>5</v>
       </c>
       <c r="DL13" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="DN13" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="DO13" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="DP13" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="DQ13" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="DR13" s="0" t="n">
         <v>10</v>
@@ -5993,16 +5996,16 @@
         <v>1</v>
       </c>
       <c r="EB13" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="EC13" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="ED13" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="EE13" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="EF13" s="0" t="n">
         <v>100</v>
@@ -6029,15 +6032,15 @@
         <v>1</v>
       </c>
       <c r="EO13" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>2</v>
@@ -6050,7 +6053,7 @@
         <v>hzb_TestP_AA_2_c-4</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>0.16</v>
@@ -6062,22 +6065,22 @@
         <v>1</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M14" s="0" t="n">
         <v>10</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O14" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P14" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q14" s="0" t="n">
         <v>100</v>
@@ -6086,7 +6089,7 @@
         <v>10</v>
       </c>
       <c r="S14" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="T14" s="0" t="n">
         <v>10</v>
@@ -6095,7 +6098,7 @@
         <v>100</v>
       </c>
       <c r="V14" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="W14" s="0" t="n">
         <v>20</v>
@@ -6104,16 +6107,16 @@
         <v>50</v>
       </c>
       <c r="Y14" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Z14" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA14" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AB14" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AC14" s="0" t="n">
         <v>1</v>
@@ -6122,7 +6125,7 @@
         <v>1</v>
       </c>
       <c r="AE14" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AF14" s="0" t="n">
         <v>2</v>
@@ -6155,7 +6158,7 @@
         <v>10</v>
       </c>
       <c r="AP14" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AQ14" s="0" t="n">
         <v>10</v>
@@ -6176,40 +6179,40 @@
         <v>100</v>
       </c>
       <c r="AW14" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AX14" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AY14" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AZ14" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BA14" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BB14" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BC14" s="0" t="n">
         <v>10</v>
       </c>
       <c r="BD14" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BE14" s="0" t="n">
         <v>1</v>
       </c>
       <c r="BF14" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BG14" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BH14" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="BI14" s="0" t="n">
         <v>10</v>
@@ -6218,10 +6221,10 @@
         <v>1</v>
       </c>
       <c r="BK14" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL14" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BM14" s="0" t="n">
         <v>5</v>
@@ -6251,19 +6254,19 @@
         <v>14</v>
       </c>
       <c r="BV14" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="BX14" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BY14" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="BZ14" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="CA14" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="CB14" s="0" t="n">
         <v>10</v>
@@ -6320,25 +6323,25 @@
         <v>3</v>
       </c>
       <c r="CT14" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="CU14" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="CV14" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="CW14" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="CX14" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="CY14" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CZ14" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="DA14" s="0" t="n">
         <v>10</v>
@@ -6374,19 +6377,19 @@
         <v>5</v>
       </c>
       <c r="DL14" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="DN14" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="DO14" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="DP14" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="DQ14" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="DR14" s="0" t="n">
         <v>10</v>
@@ -6413,16 +6416,16 @@
         <v>1</v>
       </c>
       <c r="EB14" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="EC14" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="ED14" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="EE14" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="EF14" s="0" t="n">
         <v>100</v>
@@ -6449,15 +6452,15 @@
         <v>1</v>
       </c>
       <c r="EO14" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>2</v>
@@ -6470,7 +6473,7 @@
         <v>hzb_TestP_AA_2_c-5</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>0.16</v>
@@ -6482,22 +6485,22 @@
         <v>1</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M15" s="0" t="n">
         <v>10</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O15" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P15" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q15" s="0" t="n">
         <v>100</v>
@@ -6506,7 +6509,7 @@
         <v>10</v>
       </c>
       <c r="S15" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="T15" s="0" t="n">
         <v>10</v>
@@ -6515,7 +6518,7 @@
         <v>100</v>
       </c>
       <c r="V15" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="W15" s="0" t="n">
         <v>20</v>
@@ -6524,16 +6527,16 @@
         <v>50</v>
       </c>
       <c r="Y15" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Z15" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA15" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AB15" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AC15" s="0" t="n">
         <v>1</v>
@@ -6542,7 +6545,7 @@
         <v>1</v>
       </c>
       <c r="AE15" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AF15" s="0" t="n">
         <v>2</v>
@@ -6575,7 +6578,7 @@
         <v>10</v>
       </c>
       <c r="AP15" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AQ15" s="0" t="n">
         <v>10</v>
@@ -6596,40 +6599,40 @@
         <v>100</v>
       </c>
       <c r="AW15" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AX15" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AY15" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AZ15" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BA15" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BB15" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BC15" s="0" t="n">
         <v>10</v>
       </c>
       <c r="BD15" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BE15" s="0" t="n">
         <v>1</v>
       </c>
       <c r="BF15" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BG15" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BH15" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="BI15" s="0" t="n">
         <v>10</v>
@@ -6638,10 +6641,10 @@
         <v>1</v>
       </c>
       <c r="BK15" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL15" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BM15" s="0" t="n">
         <v>5</v>
@@ -6671,19 +6674,19 @@
         <v>14</v>
       </c>
       <c r="BV15" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="BX15" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BY15" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="BZ15" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="CA15" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="CB15" s="0" t="n">
         <v>10</v>
@@ -6740,25 +6743,25 @@
         <v>3</v>
       </c>
       <c r="CT15" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="CU15" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="CV15" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="CW15" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="CX15" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="CY15" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CZ15" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="DA15" s="0" t="n">
         <v>10</v>
@@ -6794,19 +6797,19 @@
         <v>5</v>
       </c>
       <c r="DL15" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="DN15" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="DO15" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="DP15" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="DQ15" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="DR15" s="0" t="n">
         <v>10</v>
@@ -6833,16 +6836,16 @@
         <v>1</v>
       </c>
       <c r="EB15" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="EC15" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="ED15" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="EE15" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="EF15" s="0" t="n">
         <v>100</v>
@@ -6869,15 +6872,15 @@
         <v>1</v>
       </c>
       <c r="EO15" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>2</v>
@@ -6890,7 +6893,7 @@
         <v>hzb_TestP_AA_2_c-6</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>0.16</v>
@@ -6902,22 +6905,22 @@
         <v>1</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M16" s="0" t="n">
         <v>10</v>
       </c>
       <c r="N16" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O16" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P16" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q16" s="0" t="n">
         <v>100</v>
@@ -6926,7 +6929,7 @@
         <v>10</v>
       </c>
       <c r="S16" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="T16" s="0" t="n">
         <v>10</v>
@@ -6935,7 +6938,7 @@
         <v>100</v>
       </c>
       <c r="V16" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="W16" s="0" t="n">
         <v>20</v>
@@ -6944,16 +6947,16 @@
         <v>50</v>
       </c>
       <c r="Y16" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Z16" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA16" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AB16" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AC16" s="0" t="n">
         <v>1</v>
@@ -6962,7 +6965,7 @@
         <v>1</v>
       </c>
       <c r="AE16" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AF16" s="0" t="n">
         <v>2</v>
@@ -6995,7 +6998,7 @@
         <v>10</v>
       </c>
       <c r="AP16" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AQ16" s="0" t="n">
         <v>10</v>
@@ -7016,40 +7019,40 @@
         <v>100</v>
       </c>
       <c r="AW16" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AX16" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AY16" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AZ16" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BA16" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BB16" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BC16" s="0" t="n">
         <v>10</v>
       </c>
       <c r="BD16" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BE16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="BF16" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BG16" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BH16" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="BI16" s="0" t="n">
         <v>10</v>
@@ -7058,10 +7061,10 @@
         <v>1</v>
       </c>
       <c r="BK16" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL16" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BM16" s="0" t="n">
         <v>5</v>
@@ -7091,19 +7094,19 @@
         <v>14</v>
       </c>
       <c r="BV16" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="BX16" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BY16" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="BZ16" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="CA16" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="CB16" s="0" t="n">
         <v>10</v>
@@ -7160,25 +7163,25 @@
         <v>3</v>
       </c>
       <c r="CT16" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="CU16" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="CV16" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="CW16" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="CX16" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="CY16" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CZ16" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="DA16" s="0" t="n">
         <v>10</v>
@@ -7214,19 +7217,19 @@
         <v>5</v>
       </c>
       <c r="DL16" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="DN16" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="DO16" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="DP16" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="DQ16" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="DR16" s="0" t="n">
         <v>10</v>
@@ -7253,16 +7256,16 @@
         <v>1</v>
       </c>
       <c r="EB16" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="EC16" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="ED16" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="EE16" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="EF16" s="0" t="n">
         <v>100</v>
@@ -7289,15 +7292,15 @@
         <v>1</v>
       </c>
       <c r="EO16" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>2</v>
@@ -7310,7 +7313,7 @@
         <v>hzb_TestP_AA_2_c-7</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H17" s="0" t="n">
         <v>0.16</v>
@@ -7322,22 +7325,22 @@
         <v>1</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M17" s="0" t="n">
         <v>10</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O17" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P17" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q17" s="0" t="n">
         <v>100</v>
@@ -7346,7 +7349,7 @@
         <v>10</v>
       </c>
       <c r="S17" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="T17" s="0" t="n">
         <v>10</v>
@@ -7355,7 +7358,7 @@
         <v>100</v>
       </c>
       <c r="V17" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="W17" s="0" t="n">
         <v>20</v>
@@ -7364,16 +7367,16 @@
         <v>50</v>
       </c>
       <c r="Y17" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Z17" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA17" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AB17" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AC17" s="0" t="n">
         <v>1</v>
@@ -7382,7 +7385,7 @@
         <v>1</v>
       </c>
       <c r="AE17" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AF17" s="0" t="n">
         <v>2</v>
@@ -7415,7 +7418,7 @@
         <v>10</v>
       </c>
       <c r="AP17" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AQ17" s="0" t="n">
         <v>10</v>
@@ -7436,40 +7439,40 @@
         <v>100</v>
       </c>
       <c r="AW17" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AX17" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AY17" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AZ17" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BA17" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BB17" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BC17" s="0" t="n">
         <v>10</v>
       </c>
       <c r="BD17" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BE17" s="0" t="n">
         <v>1</v>
       </c>
       <c r="BF17" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BG17" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BH17" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="BI17" s="0" t="n">
         <v>10</v>
@@ -7478,10 +7481,10 @@
         <v>1</v>
       </c>
       <c r="BK17" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL17" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BM17" s="0" t="n">
         <v>5</v>
@@ -7511,19 +7514,19 @@
         <v>14</v>
       </c>
       <c r="BV17" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="BX17" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BY17" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="BZ17" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="CA17" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="CB17" s="0" t="n">
         <v>10</v>
@@ -7580,25 +7583,25 @@
         <v>3</v>
       </c>
       <c r="CT17" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="CU17" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="CV17" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="CW17" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="CX17" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="CY17" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CZ17" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="DA17" s="0" t="n">
         <v>10</v>
@@ -7634,19 +7637,19 @@
         <v>5</v>
       </c>
       <c r="DL17" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="DN17" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="DO17" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="DP17" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="DQ17" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="DR17" s="0" t="n">
         <v>10</v>
@@ -7673,16 +7676,16 @@
         <v>1</v>
       </c>
       <c r="EB17" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="EC17" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="ED17" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="EE17" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="EF17" s="0" t="n">
         <v>100</v>
@@ -7709,15 +7712,15 @@
         <v>1</v>
       </c>
       <c r="EO17" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>2</v>
@@ -7730,7 +7733,7 @@
         <v>hzb_TestP_AA_2_c-8</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H18" s="0" t="n">
         <v>0.16</v>
@@ -7742,22 +7745,22 @@
         <v>1</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M18" s="0" t="n">
         <v>10</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O18" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P18" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q18" s="0" t="n">
         <v>100</v>
@@ -7766,7 +7769,7 @@
         <v>10</v>
       </c>
       <c r="S18" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="T18" s="0" t="n">
         <v>10</v>
@@ -7775,7 +7778,7 @@
         <v>100</v>
       </c>
       <c r="V18" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="W18" s="0" t="n">
         <v>20</v>
@@ -7784,16 +7787,16 @@
         <v>50</v>
       </c>
       <c r="Y18" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Z18" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA18" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AB18" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AC18" s="0" t="n">
         <v>1</v>
@@ -7802,7 +7805,7 @@
         <v>1</v>
       </c>
       <c r="AE18" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AF18" s="0" t="n">
         <v>2</v>
@@ -7835,7 +7838,7 @@
         <v>10</v>
       </c>
       <c r="AP18" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AQ18" s="0" t="n">
         <v>10</v>
@@ -7856,40 +7859,40 @@
         <v>100</v>
       </c>
       <c r="AW18" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AX18" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AY18" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AZ18" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="BA18" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BB18" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BC18" s="0" t="n">
         <v>10</v>
       </c>
       <c r="BD18" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BE18" s="0" t="n">
         <v>1</v>
       </c>
       <c r="BF18" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BG18" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BH18" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="BI18" s="0" t="n">
         <v>10</v>
@@ -7898,10 +7901,10 @@
         <v>1</v>
       </c>
       <c r="BK18" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL18" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BM18" s="0" t="n">
         <v>5</v>
@@ -7931,19 +7934,19 @@
         <v>14</v>
       </c>
       <c r="BV18" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="BX18" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BY18" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="BZ18" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="CA18" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="CB18" s="0" t="n">
         <v>10</v>
@@ -8000,25 +8003,25 @@
         <v>3</v>
       </c>
       <c r="CT18" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="CU18" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="CV18" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="CW18" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="CX18" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="CY18" s="0" t="n">
         <v>10</v>
       </c>
       <c r="CZ18" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="DA18" s="0" t="n">
         <v>10</v>
@@ -8054,19 +8057,19 @@
         <v>5</v>
       </c>
       <c r="DL18" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="DN18" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="DO18" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="DP18" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="DQ18" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="DR18" s="0" t="n">
         <v>10</v>
@@ -8093,16 +8096,16 @@
         <v>1</v>
       </c>
       <c r="EB18" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="EC18" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="ED18" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="EE18" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="EF18" s="0" t="n">
         <v>100</v>
@@ -8129,7 +8132,7 @@
         <v>1</v>
       </c>
       <c r="EO18" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>